<commit_message>
rename the file 001
</commit_message>
<xml_diff>
--- a/分组.xlsx
+++ b/分组.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AdvancedWriting\AdvancedWriting2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03528487-1DAA-46C5-8C0B-558F9D9A7999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49037E1B-104A-4FFC-9D11-D9F49F2B4BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{15B08866-595F-47E9-BAD9-77A2D489EACF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{15B08866-595F-47E9-BAD9-77A2D489EACF}"/>
   </bookViews>
   <sheets>
     <sheet name="2122111011" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>jxl</author>
+  </authors>
+  <commentList>
+    <comment ref="A34" authorId="0" shapeId="0" xr:uid="{0603F856-16F0-425D-B8F5-ED7BCAC7DBFF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>jxl:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+3班4组</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="248">
   <si>
     <t>学生姓名</t>
   </si>
@@ -786,6 +820,10 @@
   </si>
   <si>
     <t>212241811532</t>
+  </si>
+  <si>
+    <t>title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -795,7 +833,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -811,16 +849,35 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -843,13 +900,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -869,6 +937,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1187,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C1078B-6498-4F95-93D7-0658BCA6C2A1}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="C26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1698,11 +1775,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46653091-3F9A-4DD5-9EBF-64E638960BE4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46653091-3F9A-4DD5-9EBF-64E638960BE4}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2273,53 +2350,53 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="7">
         <v>7</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="7" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="7">
         <v>7</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="7" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="7">
         <v>7</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="7" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2360,15 +2437,16 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F84D50-F66A-47F7-AF02-303300F949B4}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2379,7 +2457,7 @@
     <col min="5" max="5" width="89" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2395,8 +2473,11 @@
       <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+      <c r="F1" s="9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>159</v>
       </c>
@@ -2413,7 +2494,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>163</v>
       </c>
@@ -2430,7 +2511,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>165</v>
       </c>
@@ -2447,7 +2528,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>167</v>
       </c>
@@ -2464,7 +2545,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>169</v>
       </c>
@@ -2481,7 +2562,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>171</v>
       </c>
@@ -2498,7 +2579,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>175</v>
       </c>
@@ -2515,7 +2596,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>177</v>
       </c>
@@ -2532,7 +2613,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>179</v>
       </c>
@@ -2549,7 +2630,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>181</v>
       </c>
@@ -2566,7 +2647,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>184</v>
       </c>
@@ -2583,7 +2664,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>186</v>
       </c>
@@ -2600,7 +2681,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>188</v>
       </c>
@@ -2617,7 +2698,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>147</v>
       </c>
@@ -2634,7 +2715,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
add the paper name for each group
</commit_message>
<xml_diff>
--- a/分组.xlsx
+++ b/分组.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AdvancedWriting\AdvancedWriting2024\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8D1820-1695-4CCD-9BC9-9F5F21CE53DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="21600" windowHeight="9555"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2122111011" sheetId="1" r:id="rId1"/>
@@ -29,12 +35,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>jxl</author>
   </authors>
   <commentList>
-    <comment ref="A34" authorId="0">
+    <comment ref="A34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -580,7 +586,7 @@
     <t>英美作品分析</t>
   </si>
   <si>
-    <t>从叙事学视角看《献给艾米丽的玫瑰》
+    <t>从叙事学视角看《献给艾米丽的玫瑰》_x000D_
  "A Rose for Emily" from the perspective of Narratology</t>
   </si>
   <si>
@@ -617,7 +623,7 @@
     <t>语言学</t>
   </si>
   <si>
-    <t xml:space="preserve">研究第二语言习得的影响因素
+    <t xml:space="preserve">研究第二语言习得的影响因素_x000D_
 Thesis on the Factors in Second Language Acquisition </t>
   </si>
   <si>
@@ -645,7 +651,7 @@
     <t>212241811429</t>
   </si>
   <si>
-    <t>英美现当代文学中的女性形象演变研究
+    <t>英美现当代文学中的女性形象演变研究_x000D_
 A Study on the Evolution of Female Characters in Anglo-American Contemporary Literature</t>
   </si>
   <si>
@@ -683,7 +689,7 @@
     <t>科幻文学</t>
   </si>
   <si>
-    <t>后人类主义视角下《神经漫游者》中的身体伦理边界
+    <t>后人类主义视角下《神经漫游者》中的身体伦理边界_x000D_
 The Ethical Boundaries of the Body in “Neuromancer”from a Posthumanist Perspective</t>
   </si>
   <si>
@@ -714,12 +720,11 @@
     <t>英美文学（作品分析）</t>
   </si>
   <si>
-    <t>女性主义视角下的《傲慢与偏见》
+    <t>女性主义视角下的《傲慢与偏见》_x000D_
 “Pride and Prejudice” in Feminist Perspective</t>
   </si>
   <si>
-    <t xml:space="preserve">张楠楠-</t>
+    <t>张楠楠_x000D_</t>
   </si>
   <si>
     <t>212241811522</t>
@@ -737,7 +742,7 @@
     <t>212241811505</t>
   </si>
   <si>
-    <t>以女性主义视角解析《黄色墙纸》
+    <t>以女性主义视角解析《黄色墙纸》_x000D_
 Analysis of “The Yellow Wallpaper” from a Feminist Perspective</t>
   </si>
   <si>
@@ -771,7 +776,7 @@
     <t>212241811520</t>
   </si>
   <si>
-    <t>哥特小说中的性别政治：女性角色的演变
+    <t>哥特小说中的性别政治：女性角色的演变_x000D_
 The Sexual politics in Gothic Fiction: The Evolution of Female Characters</t>
   </si>
   <si>
@@ -808,7 +813,7 @@
     <t>跨文化比较研究</t>
   </si>
   <si>
-    <t>多模态隐喻视角下中美电影中英雄主义精神对比研究—以《战狼》与《复仇者联盟》为例
+    <t>多模态隐喻视角下中美电影中英雄主义精神对比研究—以《战狼》与《复仇者联盟》为例_x000D_
 A Comparative Study of Heroism in Chinese and American Films from the Perspective of Multimodal Metaphor: A Case Study of “Wolf Warriors” and “The Avengers”</t>
   </si>
   <si>
@@ -828,7 +833,7 @@
     <t>外语教学</t>
   </si>
   <si>
-    <t>科学技术的发展对于英语非母语学习者的帮助
+    <t>科学技术的发展对于英语非母语学习者的帮助_x000D_
 The development of science and technology to help non-native English learners</t>
   </si>
   <si>
@@ -848,171 +853,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="0_ "/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="178" formatCode="0_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1026,8 +876,14 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1040,194 +896,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1261,251 +931,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1534,71 +962,27 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1856,25 +1240,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.85" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.3362831858407" style="8" customWidth="1"/>
-    <col min="5" max="5" width="91.3362831858407" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="91.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.9" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1891,7 +1275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="27.75" spans="1:5">
+    <row r="2" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1908,7 +1292,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" ht="27.75" spans="1:5">
+    <row r="3" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1925,7 +1309,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" ht="27.75" spans="1:5">
+    <row r="4" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1942,7 +1326,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" ht="27.75" spans="1:5">
+    <row r="5" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1959,7 +1343,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" ht="27.75" spans="1:5">
+    <row r="6" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1976,7 +1360,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" ht="27.75" spans="1:5">
+    <row r="7" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1993,7 +1377,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" ht="27.75" spans="1:5">
+    <row r="8" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -2010,7 +1394,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" ht="27.75" spans="1:5">
+    <row r="9" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -2027,7 +1411,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" ht="27.75" spans="1:5">
+    <row r="10" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -2044,7 +1428,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" ht="27.75" spans="1:5">
+    <row r="11" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -2061,7 +1445,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" ht="13.9" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -2078,7 +1462,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" ht="13.9" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -2095,7 +1479,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" ht="13.9" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -2112,7 +1496,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" ht="13.9" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
@@ -2129,7 +1513,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" ht="13.9" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -2146,7 +1530,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" ht="13.9" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
@@ -2163,7 +1547,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" ht="27.75" spans="1:5">
+    <row r="18" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
@@ -2180,7 +1564,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" ht="27.75" spans="1:5">
+    <row r="19" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>49</v>
       </c>
@@ -2197,7 +1581,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" ht="27.75" spans="1:5">
+    <row r="20" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>51</v>
       </c>
@@ -2214,7 +1598,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" ht="41.65" spans="1:5">
+    <row r="21" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
@@ -2231,7 +1615,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" ht="41.65" spans="1:5">
+    <row r="22" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
@@ -2248,7 +1632,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" ht="41.65" spans="1:5">
+    <row r="23" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>59</v>
       </c>
@@ -2265,7 +1649,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" ht="41.65" spans="1:5">
+    <row r="24" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>61</v>
       </c>
@@ -2282,7 +1666,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" ht="41.65" spans="1:5">
+    <row r="25" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>63</v>
       </c>
@@ -2299,7 +1683,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" ht="27.75" spans="1:5">
+    <row r="26" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>65</v>
       </c>
@@ -2316,7 +1700,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" ht="27.75" spans="1:5">
+    <row r="27" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>67</v>
       </c>
@@ -2333,7 +1717,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" ht="27.75" spans="1:5">
+    <row r="28" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>68</v>
       </c>
@@ -2350,7 +1734,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" ht="27.75" spans="1:5">
+    <row r="29" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>69</v>
       </c>
@@ -2367,7 +1751,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" ht="27.75" spans="1:5">
+    <row r="30" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>70</v>
       </c>
@@ -2384,7 +1768,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" ht="27.75" spans="1:5">
+    <row r="31" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>73</v>
       </c>
@@ -2401,7 +1785,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" ht="27.75" spans="1:5">
+    <row r="32" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>75</v>
       </c>
@@ -2418,7 +1802,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" ht="27.75" spans="1:5">
+    <row r="33" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>77</v>
       </c>
@@ -2435,7 +1819,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" ht="27.75" spans="1:5">
+    <row r="34" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>79</v>
       </c>
@@ -2452,7 +1836,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" ht="27.75" spans="1:5">
+    <row r="35" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>81</v>
       </c>
@@ -2470,28 +1854,27 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.85" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.9115044247788" style="4" customWidth="1"/>
-    <col min="5" max="5" width="57.8318584070796" customWidth="1"/>
+    <col min="2" max="2" width="13.9140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="57.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2508,7 +1891,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>83</v>
       </c>
@@ -2525,7 +1908,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>87</v>
       </c>
@@ -2542,7 +1925,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>89</v>
       </c>
@@ -2559,7 +1942,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>91</v>
       </c>
@@ -2576,7 +1959,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>93</v>
       </c>
@@ -2593,7 +1976,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>96</v>
       </c>
@@ -2610,7 +1993,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>98</v>
       </c>
@@ -2627,7 +2010,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>100</v>
       </c>
@@ -2644,7 +2027,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>102</v>
       </c>
@@ -2661,7 +2044,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>104</v>
       </c>
@@ -2678,7 +2061,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>106</v>
       </c>
@@ -2695,7 +2078,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>109</v>
       </c>
@@ -2712,7 +2095,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>111</v>
       </c>
@@ -2729,7 +2112,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>113</v>
       </c>
@@ -2746,7 +2129,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>115</v>
       </c>
@@ -2763,7 +2146,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>117</v>
       </c>
@@ -2780,7 +2163,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>119</v>
       </c>
@@ -2797,7 +2180,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>123</v>
       </c>
@@ -2814,7 +2197,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>125</v>
       </c>
@@ -2831,7 +2214,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>127</v>
       </c>
@@ -2848,7 +2231,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>129</v>
       </c>
@@ -2865,7 +2248,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>132</v>
       </c>
@@ -2882,7 +2265,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>134</v>
       </c>
@@ -2899,7 +2282,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>136</v>
       </c>
@@ -2916,7 +2299,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>138</v>
       </c>
@@ -2933,7 +2316,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>140</v>
       </c>
@@ -2950,7 +2333,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>142</v>
       </c>
@@ -2967,7 +2350,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>145</v>
       </c>
@@ -2984,7 +2367,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>147</v>
       </c>
@@ -3001,7 +2384,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>149</v>
       </c>
@@ -3018,7 +2401,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>151</v>
       </c>
@@ -3035,7 +2418,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>153</v>
       </c>
@@ -3052,7 +2435,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>155</v>
       </c>
@@ -3069,7 +2452,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>159</v>
       </c>
@@ -3086,7 +2469,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>161</v>
       </c>
@@ -3103,7 +2486,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>163</v>
       </c>
@@ -3120,7 +2503,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>166</v>
       </c>
@@ -3138,30 +2521,29 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.85" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.8318584070796" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="21.3362831858407" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.9" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3181,7 +2563,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" ht="27.75" spans="1:5">
+    <row r="2" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>169</v>
       </c>
@@ -3198,7 +2580,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" ht="27.75" spans="1:5">
+    <row r="3" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>173</v>
       </c>
@@ -3215,7 +2597,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" ht="27.75" spans="1:5">
+    <row r="4" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>175</v>
       </c>
@@ -3232,7 +2614,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" ht="27.75" spans="1:5">
+    <row r="5" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>177</v>
       </c>
@@ -3249,7 +2631,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" ht="27.75" spans="1:5">
+    <row r="6" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>179</v>
       </c>
@@ -3266,7 +2648,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" ht="27.75" spans="1:5">
+    <row r="7" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>181</v>
       </c>
@@ -3283,7 +2665,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" ht="27.75" spans="1:5">
+    <row r="8" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>185</v>
       </c>
@@ -3300,7 +2682,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" ht="27.75" spans="1:5">
+    <row r="9" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>187</v>
       </c>
@@ -3317,7 +2699,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" ht="27.75" spans="1:5">
+    <row r="10" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>189</v>
       </c>
@@ -3334,7 +2716,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" ht="27.75" spans="1:5">
+    <row r="11" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>191</v>
       </c>
@@ -3351,7 +2733,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" ht="27.75" spans="1:5">
+    <row r="12" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>194</v>
       </c>
@@ -3368,7 +2750,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" ht="27.75" spans="1:5">
+    <row r="13" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>196</v>
       </c>
@@ -3385,7 +2767,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" ht="27.75" spans="1:5">
+    <row r="14" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>198</v>
       </c>
@@ -3402,7 +2784,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="15" ht="27.75" spans="1:5">
+    <row r="15" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>155</v>
       </c>
@@ -3419,7 +2801,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="16" ht="27.75" spans="1:5">
+    <row r="16" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>159</v>
       </c>
@@ -3436,7 +2818,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="17" ht="27.75" spans="1:5">
+    <row r="17" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>161</v>
       </c>
@@ -3453,7 +2835,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="18" ht="27.75" spans="1:5">
+    <row r="18" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>202</v>
       </c>
@@ -3470,7 +2852,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="19" ht="27.75" spans="1:5">
+    <row r="19" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>206</v>
       </c>
@@ -3487,7 +2869,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="20" ht="27.75" spans="1:5">
+    <row r="20" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>208</v>
       </c>
@@ -3504,7 +2886,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="21" ht="27.75" spans="1:5">
+    <row r="21" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>210</v>
       </c>
@@ -3521,7 +2903,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="22" ht="27.75" spans="1:5">
+    <row r="22" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>212</v>
       </c>
@@ -3538,7 +2920,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="23" ht="27.75" spans="1:5">
+    <row r="23" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>216</v>
       </c>
@@ -3555,7 +2937,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="24" ht="27.75" spans="1:5">
+    <row r="24" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>218</v>
       </c>
@@ -3572,7 +2954,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="25" ht="27.75" spans="1:5">
+    <row r="25" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>220</v>
       </c>
@@ -3589,7 +2971,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="26" ht="27.75" spans="1:5">
+    <row r="26" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>223</v>
       </c>
@@ -3606,7 +2988,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" ht="27.75" spans="1:5">
+    <row r="27" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>225</v>
       </c>
@@ -3623,7 +3005,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="28" ht="27.75" spans="1:5">
+    <row r="28" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>227</v>
       </c>
@@ -3640,7 +3022,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" ht="27.75" spans="1:5">
+    <row r="29" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>229</v>
       </c>
@@ -3657,7 +3039,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="30" ht="27.75" spans="1:5">
+    <row r="30" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>231</v>
       </c>
@@ -3674,7 +3056,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="31" ht="27.75" spans="1:5">
+    <row r="31" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>234</v>
       </c>
@@ -3691,7 +3073,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="32" ht="27.75" spans="1:5">
+    <row r="32" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>236</v>
       </c>
@@ -3708,7 +3090,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="33" ht="27.75" spans="1:5">
+    <row r="33" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>238</v>
       </c>
@@ -3725,7 +3107,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="34" ht="27.75" spans="1:5">
+    <row r="34" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>240</v>
       </c>
@@ -3742,7 +3124,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="35" ht="41.65" spans="1:5">
+    <row r="35" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>242</v>
       </c>
@@ -3759,7 +3141,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="36" ht="41.65" spans="1:5">
+    <row r="36" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>246</v>
       </c>
@@ -3776,7 +3158,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="37" ht="27.75" spans="1:5">
+    <row r="37" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>248</v>
       </c>
@@ -3793,7 +3175,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="38" ht="27.75" spans="1:5">
+    <row r="38" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>252</v>
       </c>
@@ -3810,7 +3192,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="39" ht="27.75" spans="1:5">
+    <row r="39" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>254</v>
       </c>
@@ -3828,7 +3210,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>